<commit_message>
Excel null cell value has been handel
</commit_message>
<xml_diff>
--- a/src/com/SpiceTG/TestDataFiles/UserNameAndPassword.xlsx
+++ b/src/com/SpiceTG/TestDataFiles/UserNameAndPassword.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>UserName</t>
   </si>
@@ -30,25 +30,22 @@
     <t>prasadn@leotechnosoft.net</t>
   </si>
   <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>neel.sharma@spicetg.com</t>
+  </si>
+  <si>
+    <t>spice_12345</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>mark@leotechnosoft.net</t>
+  </si>
+  <si>
     <t>leo_123</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>neel.sharma@spicetg.com</t>
-  </si>
-  <si>
-    <t>spice_12345</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>mark@leotechnosoft.net</t>
-  </si>
-  <si>
-    <t>leo_12345</t>
   </si>
 </sst>
 </file>
@@ -122,7 +119,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -134,6 +131,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -432,10 +430,15 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="5"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -453,32 +456,30 @@
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update with Failed UserName or Password Screen Shot
</commit_message>
<xml_diff>
--- a/src/com/SpiceTG/TestDataFiles/UserNameAndPassword.xlsx
+++ b/src/com/SpiceTG/TestDataFiles/UserNameAndPassword.xlsx
@@ -455,9 +455,7 @@
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
@@ -477,7 +475,9 @@
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>

</xml_diff>